<commit_message>
lagt till kommentarer till alla mina funktioner
</commit_message>
<xml_diff>
--- a/Lab3/final_scheme.xlsx
+++ b/Lab3/final_scheme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d98b1da7e90db015/Documents/BTH - Kurser/DV2626 - Maskininlärning/machinelearning/Lab3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_33FD93B6D3105D1ED7D83011595ED87656CD2F37" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A44C1853-47E1-4E10-AB34-F54572679AE7}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_1B75F2B3D320D241E3992B11595ED87656CD08BE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A87BE40-F432-4B2B-9EB5-DAB8FFA7E498}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="186">
   <si>
     <t>Day</t>
   </si>
@@ -43,435 +43,534 @@
     <t>MONDAY</t>
   </si>
   <si>
-    <t>Bench Dip</t>
-  </si>
-  <si>
-    <t>Weighted</t>
-  </si>
-  <si>
-    <t>Sit on inside of one of two benches placed parallel, slightly less than leg's length away. Place hands on edge of bench. Straighten arms, slide rear end off of edge of bench and position heels on adjacent bench with legs straight. Have assistant place weight on lap near hips.</t>
-  </si>
-  <si>
-    <t>Lower body by bending arms until slight stretch is felt in chest or shoulder, or rear end touches floor. Raise body and repeat.</t>
+    <t>Rear Delt Row</t>
+  </si>
+  <si>
+    <t>Barbell</t>
+  </si>
+  <si>
+    <t>Bend knees slightly and bend over bar with back straight, approximately horizontal. Grasp bar with wide overhand grip.</t>
+  </si>
+  <si>
+    <t>Keeping upper arm perpendicular to torso, pull barbell up toward upper chest until upper arms are just beyond horizontal. Return and repeat.</t>
+  </si>
+  <si>
+    <t>Shoulder</t>
+  </si>
+  <si>
+    <t>Presses</t>
+  </si>
+  <si>
+    <t>Cable</t>
+  </si>
+  <si>
+    <t>Lie on bench and grasp stirrups attached to low cable pulley on each side. Position stirrups out to each side of chest with bent arm under each wrist.</t>
+  </si>
+  <si>
+    <t>Push stirrups up over each shoulder until arms are straight and parallel to one another. Return stirrups to original position, until slight stretch is felt in shoulders or chest. Repeat.</t>
+  </si>
+  <si>
+    <t>Chest</t>
+  </si>
+  <si>
+    <t>Seated Reverse Fly:  pronated grip</t>
+  </si>
+  <si>
+    <t>Lever (selectorized)</t>
+  </si>
+  <si>
+    <t>Sit in machine with chest against pad. Grasp parallel handles from inside with thumbs down at shoulder height.</t>
+  </si>
+  <si>
+    <t>Keeping elbows pointed high, pull handles apart and to rear until elbows are just behind back. Return and repeat.</t>
+  </si>
+  <si>
+    <t>Shoulder External Rotation</t>
+  </si>
+  <si>
+    <t>Lever (plate loaded)</t>
+  </si>
+  <si>
+    <t>Stand or sit with side against chest height platform. With dumbbell in hand, position upper arm horizontally on platform, elbow bent so forearm is upright.</t>
+  </si>
+  <si>
+    <t>Lower dumbbell forward by rotating shoulder. Return and repeat. Continue with opposite arm.</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Incline Lateral Raise</t>
+  </si>
+  <si>
+    <t>Dumbbell</t>
+  </si>
+  <si>
+    <t>Grasp dumbbell in one hand. Lie on 30° to 45° incline bench with opposite side of body on incline, arm over top of bench, lower leg positioned on front side of seat, and upper leg on back side of seat. Position dumbbell inside of lower leg, just in front of upper leg.</t>
+  </si>
+  <si>
+    <t>With elbows slightly bent, raise arms upward and outward to sides in Y configuration until elbows are approximately lateral to each ear. Lower stirrups forward and downward in reverse pattern. Repeat.</t>
+  </si>
+  <si>
+    <t>Lying Triceps Extension:  Skull Crusher</t>
+  </si>
+  <si>
+    <t>Lie on bench with narrow overhand grip on barbell. Position barbell over shoulders with arms extended.</t>
+  </si>
+  <si>
+    <t>Lower bar to forehead by bending elbows. Extend arms and repeat.</t>
   </si>
   <si>
     <t>Triceps</t>
   </si>
   <si>
-    <t xml:space="preserve">Chest Dip </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assisted  Chest Dip  </t>
-  </si>
-  <si>
-    <t>Mountwide dip barwith oblique grip (bar diagonal under palm), arms straight with shoulders above hands. Step down onto assistance lever with hips and knees bent.</t>
-  </si>
-  <si>
-    <t>Lower body by bending arms, allowing elbows to flare out to sides. When slight stretch is felt in chest or shoulders, push body up until arms are straight. Repeat.</t>
-  </si>
-  <si>
-    <t>Chest</t>
-  </si>
-  <si>
-    <t>Inverted Shrug</t>
+    <t>Push-up:  on knees</t>
   </si>
   <si>
     <t>Body Weight</t>
   </si>
   <si>
-    <t>Stand between parallel bars. Squat down and grasp parallel bars from above. Kick legs up inverting and balancing body upside down. Legs can be kept bent or straight, positioned vertically.</t>
-  </si>
-  <si>
-    <t>Raise body up a high as possible by pulling shoulders toward ears. Lower body to original position and repeat.</t>
-  </si>
-  <si>
-    <t>Back</t>
+    <t>Lie prone on floor with hands slightly wider than shoulder width. Bend knees and raise body up off floor by extending arms with body straight.</t>
+  </si>
+  <si>
+    <t>Keeping body straight and knees bent, lower body to floor by bending arms. Push body up until arms are extended. Repeat.</t>
+  </si>
+  <si>
+    <t>Full Can Lateral Raise</t>
+  </si>
+  <si>
+    <t>Grasp dumbbells with each hand with palms facing forward.</t>
+  </si>
+  <si>
+    <t>Raise arms to side with thumb side up. Lower and repeat.</t>
+  </si>
+  <si>
+    <t>TUESDAY</t>
+  </si>
+  <si>
+    <t>Lateral Raise:  other machine</t>
+  </si>
+  <si>
+    <t>Sit in machine. Situate bent arms between padded lever and sides of body. Grasp handles if available.</t>
+  </si>
+  <si>
+    <t>Raise arms to sides until upper arms are horizontal. Return and repeat.</t>
+  </si>
+  <si>
+    <t>Fly</t>
+  </si>
+  <si>
+    <t>Grasp two dumbbells. Lie supine on bench. Support dumbbells above chest with arms fixed in slightly bent position. Internally rotate shoulders so elbows point out to sides.</t>
+  </si>
+  <si>
+    <t>Lower dumbbells to sides until chest muscles are stretched with elbows fixed in slightly bent position. Bring dumbbells together in wide hugging motion until dumbbells are nearly together. Repeat.</t>
+  </si>
+  <si>
+    <t>Front Raise:  Alternating</t>
+  </si>
+  <si>
+    <t>Stand with low double pulleys behind. Grasp stirrup attachments, one in each hand. Stand away from pulley slightly with arms back somewhat at side and elbows straight or slightly bent.</t>
+  </si>
+  <si>
+    <t>Raise one stirrup forward and upward until upper arm is well above horizontal. Lower and repeat with opposite arm, alternating between arms.</t>
+  </si>
+  <si>
+    <t>Seated Row (no chest pad):  Straight Back</t>
+  </si>
+  <si>
+    <t>Sit on seat and grasp handles with each hand. Place feet on vertically angled platform. Slide hips back with knees slightly bent.</t>
+  </si>
+  <si>
+    <t>Pull handles to waist while straightening torso upright. Pull shoulders back and push chest forward while arching back. Return until arms are extended, shoulders are stretched forward, and lower back is flexed forward. Repeat.</t>
+  </si>
+  <si>
+    <t>Rear Lateral Raise</t>
+  </si>
+  <si>
+    <t>Stand with cable columns to each side. Grasp left stirrup with right hand and right stirrup with left hand. Bend knees and bend over at hips, so torso is approximately horizontal with back straight. Point elbows outward with arms slightly bent.</t>
+  </si>
+  <si>
+    <t>Raise upper arms to sides until elbows are shoulder height. Maintain upper arms perpendicular to torso and slight bend in elbows as arms are raised to sides. Lower and repeat.</t>
+  </si>
+  <si>
+    <t>Close Grip Push-up:  on knees</t>
+  </si>
+  <si>
+    <t>Lie prone on floor with hands under shoulders or slightly narrower. Position body up off floor with extended arms and body straight.</t>
+  </si>
+  <si>
+    <t>Keeping body straight, lower body to floor by bending arms. Push body up until arms are extended. Repeat.</t>
+  </si>
+  <si>
+    <t>Chest Press</t>
+  </si>
+  <si>
+    <t>Sit on seat with chest approximately height of handles. Grasp handles with wide overhand grip; elbows out to sides just below shoulders.</t>
+  </si>
+  <si>
+    <t>Press levers until arms are extended. Return weight until chest muscles are slightly stretched. Repeat.</t>
+  </si>
+  <si>
+    <t>Lateral Raise</t>
+  </si>
+  <si>
+    <t>With low pulleys to each side, grasp left stirrup with right hand and right stirrup with left hand. Stand upright.</t>
+  </si>
+  <si>
+    <t>With elbows slightly bent, raise arms to sides   until elbows are shoulder height. Lower and repeat.</t>
+  </si>
+  <si>
+    <t>WEDNESDAY</t>
+  </si>
+  <si>
+    <t>Front Raise:  One Arm</t>
+  </si>
+  <si>
+    <t>Grasp stirrup attachment. Stand away from pulley slightly with arm back somewhat at side and elbow straight or slightly bent.</t>
+  </si>
+  <si>
+    <t>Raise stirrup forward and upward until upper arm is well above horizontal. Lower and repeat. Repeat with opposite arm.</t>
+  </si>
+  <si>
+    <t>Decline Push-up</t>
+  </si>
+  <si>
+    <t>Kneel on floor with bench or elevation behind body. Position hands on floor slightly wider than shoulder width. Place feet on bench or elevation. Raise body in plank position with body straight and arms extended.</t>
+  </si>
+  <si>
+    <t>Keeping body straight, lower upper body to floor by bending arms. To allow for full descent, pull head back slightly without arching back. Push body up until arms are extended. Repeat.</t>
+  </si>
+  <si>
+    <t>Seated Rear Delt Row</t>
+  </si>
+  <si>
+    <t>Place seat at low position. Sit on seat with chest against pad and grasp upper handles.</t>
+  </si>
+  <si>
+    <t>Pull lever with elbows up out to sides until upper arms are just beyond parallel, keeping upper arm horizontal, perpendicular to torso. Return and repeat.</t>
+  </si>
+  <si>
+    <t>Inverted Row:  On Hips</t>
+  </si>
+  <si>
+    <t>Lay on back with belly under fixed horizontal bar. Bend knees and position feet on floor. Grasp bar with wide overhand grip.</t>
+  </si>
+  <si>
+    <t>Keeping hips on floor and low back straight, pull torso up to bar. Pull shoulders back at top of movement with chest high. Return until arms are extended and shoulders are stretched forward. Repeat.</t>
+  </si>
+  <si>
+    <t>Front Raise</t>
+  </si>
+  <si>
+    <t>Grasp barbell with overhand grip with elbows straight or slightly bent.</t>
+  </si>
+  <si>
+    <t>Raise barbell forward and upward until upper arms are above horizontal. Lower and repeat.</t>
+  </si>
+  <si>
+    <t>Triceps Dip</t>
+  </si>
+  <si>
+    <t>Assisted</t>
+  </si>
+  <si>
+    <t>Mountshoulder width dip bar, arms straight with shoulders above hands. Step down onto assistance lever. Keep hips and knees straight.</t>
+  </si>
+  <si>
+    <t>Lower body until slight stretch is felt in shoulders. Push body up until arms are straight. Repeat.</t>
+  </si>
+  <si>
+    <t>Bench Press</t>
+  </si>
+  <si>
+    <t>Lie supine on bench. Dismount barbell from rack over upper chest using wide oblique overhand grip.</t>
+  </si>
+  <si>
+    <t>Lower weight to chest. Press bar upward until arms are extended. Repeat.</t>
+  </si>
+  <si>
+    <t>Shoulder Press</t>
+  </si>
+  <si>
+    <t>Stand between two low to medium height pulleys. Grasp cable stirrups from each side. Position stirrups to each side of shoulders with elbows down to sides and stirrups above or slightly narrower than elbows.</t>
+  </si>
+  <si>
+    <t>Push stirrups upward until arms are extended overhead. Return stirrups to sides of shoulders and repeat.</t>
+  </si>
+  <si>
+    <t>THURSDAY</t>
+  </si>
+  <si>
+    <t>Lateral Raise:  One Arm</t>
+  </si>
+  <si>
+    <t>Grasp stirrup cable attachment. Stand facing with side of resting arm toward low pulley. Grasp ballet bar if available.</t>
+  </si>
+  <si>
+    <t>With elbow slightly bent, raise arm to side away from low pulley until elbow is shoulder height. Lower and repeat.</t>
+  </si>
+  <si>
+    <t>Incline Bench Press</t>
+  </si>
+  <si>
+    <t>Lie supine on incline bench. Dismount barbell from rack over upper chest using wide oblique overhand grip.</t>
+  </si>
+  <si>
+    <t>Lower weight to upper chest. Press bar until arms are extended. Repeat.</t>
+  </si>
+  <si>
+    <t>Reverse Fly</t>
+  </si>
+  <si>
+    <t>Stand facing twin pulley cables positioned close together and approximately shoulder height. Grasp stirrup cable attachment in each hand. Step back away from machine so cable is taut. Stand with feet staggered. Point elbows outward with arms straight or slightly bent.</t>
+  </si>
+  <si>
+    <t>Pull stirrups out to sides, maintaining stiff elbow position throughout exercise. Return to original position and repeat.</t>
+  </si>
+  <si>
+    <t>One Arm Pull-up New!</t>
+  </si>
+  <si>
+    <t>Step up and grasp bar with underhand shoulder width grip.</t>
+  </si>
+  <si>
+    <t>Pull body up until elbows are to sides. Lower body until arms and shoulders are fully extended. Repeat.</t>
+  </si>
+  <si>
+    <t>Military Press</t>
+  </si>
+  <si>
+    <t>Grasp barbell from rack orcleanbarbell from floor with overhand grip, slightly wider than shoulder width. Position bar in front of neck.</t>
+  </si>
+  <si>
+    <t>Press bar upward until arms are extended overhead. Lower to front of neck and repeat.</t>
+  </si>
+  <si>
+    <t>Bent-over Triceps Extension</t>
+  </si>
+  <si>
+    <t>Sit on utility weight bench with barbell. Position barbell overhead with narrow overhand grip.</t>
+  </si>
+  <si>
+    <t>Lower barbell behind upper shoulders by flexing elbows allowing forearms to travel behind upper arms with elbows remaining overhead. Raise barbell overhead by extending elbows until arms are positioned straight and vertical. Lower and repeat.</t>
+  </si>
+  <si>
+    <t>Flies:  Standing Fly</t>
+  </si>
+  <si>
+    <t>Grasp two opposing high pulley dumbbell attachments. Stand with pulleys to each side. Bend over slightly by flexing hips and knees. Bend elbows slightly and internally rotate shoulders so elbows are back initially.</t>
+  </si>
+  <si>
+    <t>Bring cable attachments together in hugging motion with elbows in fixed position. Keep shoulders internally rotated so elbows are pointed upward at top and out to sides at bottom. Return to starting position until chest muscles are stretched. Repeat.</t>
+  </si>
+  <si>
+    <t>Reclined Shoulder Press</t>
+  </si>
+  <si>
+    <t>Lie on back pad facing up. Grasp lever handles on each side with overhand grip.</t>
+  </si>
+  <si>
+    <t>Press lever until arms are extended. Lower and repeat.</t>
+  </si>
+  <si>
+    <t>FRIDAY</t>
+  </si>
+  <si>
+    <t>Seated Rear Lateral Raise</t>
+  </si>
+  <si>
+    <t>Sit on edge of bench with feet placed beyond knees. Bend over and rest torso on thighs. Grasp dumbbells with each hand under legs. Position elbows with slight bend with palms facing together behind ankles (as shown) or just to sides of ankles.</t>
+  </si>
+  <si>
+    <t>Raise upper arms to sides until elbows are shoulder height. Maintain upper arms perpendicular to torso and fixed elbow position (10° to 30° angle) throughout exercise. Maintain elbows height above wrists by raising "pinkie finger" side up. Lower and repeat.</t>
+  </si>
+  <si>
+    <t>Presses:  Decline Chest Press</t>
+  </si>
+  <si>
+    <t>Sit on seat and grasp stirrups to each side. Position elbows out to sides, slightly lower than shoulder height. Position hands slightly narrower than elbow width in front of upper arms.</t>
+  </si>
+  <si>
+    <t>Push stirrups forward and slightly downward until arms are straight and parallel to one another. Return stirrups to original position, until slight stretch is felt in shoulders or chest. Repeat.</t>
+  </si>
+  <si>
+    <t>Rear Delt Inverted Row (on hips)</t>
+  </si>
+  <si>
+    <t>Lay on back with belly under fixed horizontal bar. Bend knees and position feet on floor. Grasp bar with wide overhand grip. Turn elbows outward to sides.</t>
+  </si>
+  <si>
+    <t>Keeping hips on floor, low back straight, and elbow pointed out to sides; pull torso up to bar. Return when upper arms are just beyond parallel to one another. Lower body downward until arms are extended straight. Return and repeat.</t>
+  </si>
+  <si>
+    <t>Pull-up (open-centered bar)</t>
+  </si>
+  <si>
+    <t>Assisted (machine)</t>
+  </si>
+  <si>
+    <t>Step up and grasp bar with wide overhand grip. Kneel on padded platform and lower body down with arm extended.</t>
+  </si>
+  <si>
+    <t>Pull body up until neck reaches height of hands. Lower body until arms and shoulders are fully extended. Repeat.</t>
+  </si>
+  <si>
+    <t>Arnold Press</t>
+  </si>
+  <si>
+    <t>Stand with two dumbbells position in front of shoulders, palms facing body and elbows under wrists.</t>
+  </si>
+  <si>
+    <t>Initiate movement by bringing elbows out to sides. Continue to raise elbows outward while pressing dumbbells overhead until arms are straight. Lower to front of shoulders in opposite pattern and repeat.</t>
+  </si>
+  <si>
+    <t>Pushdown</t>
+  </si>
+  <si>
+    <t>Face high pulley and grasp cable attachment with narrow overhand grip. Position elbows to side.</t>
+  </si>
+  <si>
+    <t>Extend arms down. Return until forearm is close to upper arm. Repeat.</t>
+  </si>
+  <si>
+    <t>Push-up:  Archer</t>
+  </si>
+  <si>
+    <t>Lie prone with forefeet on floor and hands slightly wider than shoulder width. Raise body up off floor by extending arms with body straight.</t>
+  </si>
+  <si>
+    <t>Lying Lateral Raise</t>
+  </si>
+  <si>
+    <t>Lie on side with legs separated for support. Grasp dumbbell in front of thigh.</t>
+  </si>
+  <si>
+    <t>Raise dumbbell from floor until arm is vertical. Maintain fixed elbow position (10° to 30° angle) throughout exercise. Lower and repeat.</t>
+  </si>
+  <si>
+    <t>SATURDAY</t>
+  </si>
+  <si>
+    <t>Y Raise</t>
+  </si>
+  <si>
+    <t>Stand facing between low pulleys medium width apart, grasp left stirrup with right hand and right stirrup with left hand. Step back slightly away from pulleys and stand upright with cables crossed in front of hips.</t>
+  </si>
+  <si>
+    <t>Incline Chest Press</t>
+  </si>
+  <si>
+    <t>Sit on seat and grasp stirrups to each side (attached to medium height pulleys). Position elbows out to sides, slightly lower than shoulder height. Position hands back approximately shoulder height and elbow width.</t>
+  </si>
+  <si>
+    <t>Push stirrups away from body, slightly upward at 30º to 45º until arms are straight and parallel to one another. Return stirrups to original position until slight stretch is felt in chest or shoulders. Repeat.</t>
+  </si>
+  <si>
+    <t>Lying Rear Lateral Raise</t>
+  </si>
+  <si>
+    <t>Lie on machine with chest against padding. Position arms between padded lever arms with elbows below shoulders.</t>
+  </si>
+  <si>
+    <t>Pull arms up until elbows are beyond back. Return and repeat.</t>
+  </si>
+  <si>
+    <t>Parallel Close Grip Pull-up</t>
+  </si>
+  <si>
+    <t>Step up and grasp parallel grips. Kneel on padded platform and lower body down with arm extended.</t>
+  </si>
+  <si>
+    <t>Rear Delt Inverted Row (high bar)</t>
+  </si>
+  <si>
+    <t>Stand facing horizontal bar positioned lower to upper chest height. Step toward bar so chest makes contact. Grasp bar with wide overhand grip. Raise elbows up to shoulder height. Place feet forward on floor so body is reclined back with legs, hips and spine straight.</t>
+  </si>
+  <si>
+    <t>Lower body while keeping body straight, elbows high, and upper arms perpendicular to torso, until arms are extended straight. Pull shoulders toward bar while keeping elbows up high until upper arms are parallel to one another, or just beyond. Repeat.</t>
+  </si>
+  <si>
+    <t>Pushdown:  One Arm</t>
+  </si>
+  <si>
+    <t>Grasp dumbbell cable attachment with underhand grip. Position elbow to side.</t>
+  </si>
+  <si>
+    <t>Extend arm down. Return until forearm is close to upper arm. Repeat. Continue with opposite arm.</t>
   </si>
   <si>
     <t>Flies</t>
   </si>
   <si>
-    <t>Cable</t>
-  </si>
-  <si>
     <t>Grasp two opposing low pulley stirrup attachments. Lie supine on bench, in middle and perpendicular to both pulleys. Slightly bend elbows and internally rotate shoulders so elbows are back.</t>
   </si>
   <si>
     <t>Bring cable attachments together in hugging motion with elbows in fixed position and shoulders internally rotated so elbows are to sides. Return to starting position until slight stretch. Repeat.</t>
   </si>
   <si>
-    <t>Military Press</t>
-  </si>
-  <si>
-    <t>Barbell</t>
-  </si>
-  <si>
-    <t>Grasp barbell from rack orcleanbarbell from floor with overhand grip, slightly wider than shoulder width. Position bar in front of neck.</t>
-  </si>
-  <si>
-    <t>Press bar upward until arms are extended overhead. Lower to front of neck and repeat.</t>
-  </si>
-  <si>
-    <t>Shoulder</t>
-  </si>
-  <si>
-    <t>Incline Lateral Raise</t>
-  </si>
-  <si>
-    <t>Dumbbell</t>
-  </si>
-  <si>
-    <t>Grasp dumbbell in one hand. Lie on 30° to 45° incline bench with opposite side of body on incline, arm over top of bench, lower leg positioned on front side of seat, and upper leg on back side of seat. Position dumbbell inside of lower leg, just in front of upper leg.</t>
-  </si>
-  <si>
-    <t>With elbows slightly bent, raise arms upward and outward to sides in Y configuration until elbows are approximately lateral to each ear. Lower stirrups forward and downward in reverse pattern. Repeat.</t>
-  </si>
-  <si>
-    <t>Reverse Fly</t>
-  </si>
-  <si>
-    <t>Stand facing twin pulley cables positioned close together and approximately shoulder height. Grasp stirrup cable attachment in each hand. Step back away from machine so cable is taut. Stand with feet staggered. Point elbows outward with arms straight or slightly bent.</t>
-  </si>
-  <si>
-    <t>Pull stirrups out to sides, maintaining stiff elbow position throughout exercise. Return to original position and repeat.</t>
-  </si>
-  <si>
-    <t>Y Raise</t>
-  </si>
-  <si>
-    <t>Stand facing between low pulleys medium width apart, grasp left stirrup with right hand and right stirrup with left hand. Step back slightly away from pulleys and stand upright with cables crossed in front of hips.</t>
-  </si>
-  <si>
-    <t>TUESDAY</t>
-  </si>
-  <si>
-    <t>Triceps Dip</t>
-  </si>
-  <si>
-    <t>Assisted</t>
-  </si>
-  <si>
-    <t>Mountshoulder width dip bar, arms straight with shoulders above hands. Step down onto assistance lever. Keep hips and knees straight.</t>
-  </si>
-  <si>
-    <t>Lower body until slight stretch is felt in shoulders. Push body up until arms are straight. Repeat.</t>
-  </si>
-  <si>
-    <t>Push-up Plus</t>
-  </si>
-  <si>
-    <t>Lie supine on incline bench with shoulders under bar. Grasp bar with shoulder width overhand grip. Extend elbows. Disengage bar by rotating bar back.</t>
+    <t>Seated Rear Delt Row:  alternative machine</t>
+  </si>
+  <si>
+    <t>SUNDAY</t>
+  </si>
+  <si>
+    <t>Front Lateral Raise</t>
+  </si>
+  <si>
+    <t>Grasp dumbbell cable attachment. Stand facing side with resting arm toward low pulley. Grasp ballet bar if available for support. Internally rotate shoulders so elbows point out to sides.</t>
+  </si>
+  <si>
+    <t>With elbow straight or slightly bent, raise upper arm away from low pulley to side, slightly to front (30°) until upper arm is shoulder height. Lower and repeat. Continue with opposite arm.</t>
+  </si>
+  <si>
+    <t>Incline Fly</t>
+  </si>
+  <si>
+    <t>Sit on seat with stirrups in each hand (attached to low cable pulleys). Lie back on incline back support. Position stirrups out to each side of chest with bent arm under each wrist. Press stirrups over each shoulder until arms vertical. Bend elbows slightly and internally rotate shoulders so elbows point out to sides.</t>
+  </si>
+  <si>
+    <t>Lower stirrups outward to sides of shoulders. Keep elbows fixed in slightly bent position. When a stretch is felt in chest or shoulders, bring stirrups back together in hugging motion above upper chest until stirrups are nearly together Repeat.</t>
+  </si>
+  <si>
+    <t>Upright Row</t>
+  </si>
+  <si>
+    <t>Grasp bar with shoulder width or slightly narrower overhand grip.</t>
+  </si>
+  <si>
+    <t>Pull bar to neck with elbows leading. Allow wrists to flex as bar rises. Lower and repeat.</t>
+  </si>
+  <si>
+    <t>Pullover</t>
+  </si>
+  <si>
+    <t>Lie upper back perpendicular on bench. Flex hips slightly. Grasp barbell from behind and position over chest with elbows bent slightly.</t>
+  </si>
+  <si>
+    <t>With elbows bent slightly, lower bar over and beyond head until shoulders are fully flexed or upper arms are approximately parallel to torso. Return and repeat.</t>
+  </si>
+  <si>
+    <t>Military Press:  Seated</t>
+  </si>
+  <si>
+    <t>Grasp barbell with slightly wider than shoulder width overhand grip from rack. Position bar near upper chest.</t>
+  </si>
+  <si>
+    <t>Press bar upward until arms are extended overhead. Return to upper chest and repeat.</t>
+  </si>
+  <si>
+    <t>Triceps Extension</t>
+  </si>
+  <si>
+    <t>Incline Shoulder Raise</t>
+  </si>
+  <si>
+    <t>Lie supine on incline bench. Dismount barbell from rack with shoulder width overhand grip. Position barbell over upper chest with elbows extended.</t>
   </si>
   <si>
     <t>Raise shoulders toward bar as high as possible. Lower shoulders to bench and repeat.</t>
   </si>
   <si>
-    <t>Seated Rows (Others)</t>
-  </si>
-  <si>
-    <t>Lever (plate loaded)</t>
-  </si>
-  <si>
-    <t>Sit on seat and position chest against pad. Grasp lever handles with overhand/neutral grip.</t>
-  </si>
-  <si>
-    <t>Pull levers back until elbows are behind back and shoulders are pulled back. Return until arms are extended and shoulders are stretched forward. Repeat.</t>
-  </si>
-  <si>
-    <t>Presses:  Bench Press</t>
-  </si>
-  <si>
-    <t>Lie on bench and grasp stirrups attached to low cable pulley on each side. Position stirrups out to each side of chest with bent arm under each wrist.</t>
-  </si>
-  <si>
-    <t>Push stirrups up over each shoulder until arms are straight and parallel to one another. Return stirrups to original position, until slight stretch is felt in shoulders or chest. Repeat.</t>
-  </si>
-  <si>
-    <t>Shoulder Press:  Seated</t>
-  </si>
-  <si>
-    <t>Sit on seat and grasp stirrups from low to medium low position from each side. Position stirrups to each side of shoulders with elbows down to sides and stirrups above or slightly narrower than elbows.</t>
-  </si>
-  <si>
-    <t>Push stirrups upward until arms are extended overhead. Return stirrups to sides of shoulders and repeat.</t>
-  </si>
-  <si>
-    <t>Shoulder Press</t>
-  </si>
-  <si>
-    <t>Stand between two low to medium height pulleys. Grasp cable stirrups from each side. Position stirrups to each side of shoulders with elbows down to sides and stirrups above or slightly narrower than elbows.</t>
-  </si>
-  <si>
-    <t>Seated Reverse Fly</t>
-  </si>
-  <si>
-    <t>Lever (selectorized)</t>
-  </si>
-  <si>
-    <t>Sit on machine with chest against pad. Grasp parallel handles with thumbs up at shoulder height. Slightly bend elbows and internally rotate shoulders so elbows are also at height of shoulders.</t>
-  </si>
-  <si>
-    <t>Keeping elbows pointed high, pull handles apart and to rear until elbows are just behind back. Return and repeat.</t>
-  </si>
-  <si>
-    <t>WEDNESDAY</t>
-  </si>
-  <si>
-    <t>Incline Bench Press</t>
-  </si>
-  <si>
-    <t>Lie supine on incline bench. Dismount barbell from rack over upper chest using wide oblique overhand grip.</t>
-  </si>
-  <si>
-    <t>Lower weight to upper chest. Press bar until arms are extended. Repeat.</t>
-  </si>
-  <si>
-    <t>Inverted Row</t>
-  </si>
-  <si>
-    <t>Sit on seat and position chest against pad. Grasp lever handles with underhand grip.</t>
-  </si>
-  <si>
-    <t>Incline Chest Press</t>
-  </si>
-  <si>
-    <t>Sit on seat and grasp stirrups to each side (attached to medium height pulleys). Position elbows out to sides, slightly lower than shoulder height. Position hands back approximately shoulder height and elbow width.</t>
-  </si>
-  <si>
-    <t>Push stirrups away from body, slightly upward at 30º to 45º until arms are straight and parallel to one another. Return stirrups to original position until slight stretch is felt in chest or shoulders. Repeat.</t>
-  </si>
-  <si>
-    <t>Upright Row​​​​​​​</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Stand behind bar mid-thigh height. Grasp bar with shoulder width or slightly narrower overhand grip. Disengage bar by rotating bar back and stand upright.</t>
-  </si>
-  <si>
-    <t>Pull bar to neck with elbows leading. Allow wrists to flex as bar rises. Lower and repeat.</t>
-  </si>
-  <si>
-    <t>Seated Rear Lateral Raise</t>
-  </si>
-  <si>
-    <t>Sit on edge of bench with feet placed beyond knees. Bend over and rest torso on thighs. Grasp dumbbells with each hand under legs. Position elbows with slight bend with palms facing together behind ankles (as shown) or just to sides of ankles.</t>
-  </si>
-  <si>
-    <t>Raise upper arms to sides until elbows are shoulder height. Maintain upper arms perpendicular to torso and fixed elbow position (10° to 30° angle) throughout exercise. Maintain elbows height above wrists by raising "pinkie finger" side up. Lower and repeat.</t>
-  </si>
-  <si>
-    <t>THURSDAY</t>
-  </si>
-  <si>
-    <t>Triceps Extension:  with preacher pad New!</t>
-  </si>
-  <si>
-    <t>Sit on seat. Grasp handles and place back of upper arms parallel on padding with elbows approximately in line with lever's fulcrum.</t>
-  </si>
-  <si>
-    <t>Push lever down until arms are fully extended. Return until forearms contact upper arms. Repeat.</t>
-  </si>
-  <si>
-    <t>Push-up</t>
-  </si>
-  <si>
-    <t>Lie prone on floor with hands slightly wider than shoulder width. Raise body up off floor by extending arms with body straight. Partner can place weight plate(s) on back if needed.</t>
-  </si>
-  <si>
-    <t>Keeping body straight, lower body to floor by bending arms. Push body up until arms are extended. Repeat.</t>
-  </si>
-  <si>
-    <t>Inverted Row:  High Bar</t>
-  </si>
-  <si>
-    <t>Stand facing arms length away from waist to head height horizontal bar. Grasp bar with wide overhand grip. Position body under bar with legs, hips and spine straight. Arms should be straight, approximately perpendicular to body. Heels should make contact with floor.</t>
-  </si>
-  <si>
-    <t>Keeping body straight, pull body up to bar. Pull shoulders back at top of movement with chest high. Return until arms are extended and shoulders are stretched forward. Repeat.</t>
-  </si>
-  <si>
-    <t>Flies:  Seated Fly</t>
-  </si>
-  <si>
-    <t>Sit on seat and grasp stirrups to each side. Slightly bend elbows and internally rotate shoulders so elbows are back.</t>
-  </si>
-  <si>
-    <t>Keeping elbows pointed high, bring cable attachments together in hugging motion with elbows in fixed position. Return to starting position until slight stretch. Repeat.</t>
-  </si>
-  <si>
-    <t>Pike Press (between benches)</t>
-  </si>
-  <si>
-    <t>Kneel on two benches positioned side by side slightly apart at end nearest head. Place hands on ends of benches. With forefeet on opposite ends of bench, raise rear end high up with arms, back, and knees straight. Adjust feet so they are somewhat close to hands while keeping back and legs straight.</t>
-  </si>
-  <si>
-    <t>Lower head between ends of benches by bending arms. Push body back up to original position by extending arms. Repeat.</t>
-  </si>
-  <si>
-    <t>FRIDAY</t>
-  </si>
-  <si>
-    <t>Chest Dip</t>
-  </si>
-  <si>
-    <t>Shrug with Stirrups</t>
-  </si>
-  <si>
-    <t>Stand between two low pulleys and grasp stirrups to each side. Stand upright with arms straight down to each side.</t>
-  </si>
-  <si>
-    <t>With arms straight, elevate shoulders as high as possible. Lower and repeat.</t>
-  </si>
-  <si>
-    <t>Decline Bench Press</t>
-  </si>
-  <si>
-    <t>Lie supine on decline bench with feet under leg brace. Dismount barbell from rack over chest using wide oblique overhand grip.</t>
-  </si>
-  <si>
-    <t>Lower weight to chest. Press bar until arms are extended. Repeat.</t>
-  </si>
-  <si>
-    <t>Lateral Raise:  other machine</t>
-  </si>
-  <si>
-    <t>Sit in machine. Situate bent arms between padded lever and sides of body. Grasp handles if available.</t>
-  </si>
-  <si>
-    <t>Raise arms to sides until upper arms are horizontal. Return and repeat.</t>
-  </si>
-  <si>
-    <t>Front Raise</t>
-  </si>
-  <si>
-    <t>Grasp barbell with overhand grip with elbows straight or slightly bent.</t>
-  </si>
-  <si>
-    <t>Raise barbell forward and upward until upper arms are above horizontal. Lower and repeat.</t>
-  </si>
-  <si>
-    <t>Front Raise:  One Arm</t>
-  </si>
-  <si>
-    <t>Grasp stirrup attachment. Stand away from pulley slightly with arm back somewhat at side and elbow straight or slightly bent.</t>
-  </si>
-  <si>
-    <t>Raise stirrup forward and upward until upper arm is well above horizontal. Lower and repeat. Repeat with opposite arm.</t>
-  </si>
-  <si>
-    <t>Shoulder Press:  One Arm</t>
-  </si>
-  <si>
-    <t>Stand with dumbbells positioned near shoulder with elbow below wrists.</t>
-  </si>
-  <si>
-    <t>Press dumbbell upward until arm is extended overhead. Lower to side of shoulder and repeat.</t>
-  </si>
-  <si>
-    <t>SATURDAY</t>
-  </si>
-  <si>
-    <t>Pulldown</t>
-  </si>
-  <si>
-    <t>Grasp cable bar with wide grip. Sit with thighs under supports.</t>
-  </si>
-  <si>
-    <t>Pull down cable bar to upper chest. Return until arms and shoulders are fully extended. Repeat.</t>
-  </si>
-  <si>
-    <t>Flies:  Lying Fly</t>
-  </si>
-  <si>
-    <t>Lying Lateral Raise</t>
-  </si>
-  <si>
-    <t>Lie on side with legs separated for support. Grasp dumbbell in front of thigh.</t>
-  </si>
-  <si>
-    <t>Raise dumbbell from floor until arm is vertical. Maintain fixed elbow position (10° to 30° angle) throughout exercise. Lower and repeat.</t>
-  </si>
-  <si>
-    <t>Rear Delt Row</t>
-  </si>
-  <si>
-    <t>Bend knees slightly and bend over bar with back straight, approximately horizontal. Grasp bar with wide overhand grip.</t>
-  </si>
-  <si>
-    <t>Keeping upper arm perpendicular to torso, pull barbell up toward upper chest until upper arms are just beyond horizontal. Return and repeat.</t>
-  </si>
-  <si>
-    <t>Upright Row:  with rope</t>
-  </si>
-  <si>
-    <t>Grasp each side of rope with overhand grip, just under rope ends. Stand close to pulley.</t>
-  </si>
-  <si>
-    <t>Pull rope ends to front of shoulders with elbows leading. Allow wrists to flex as stirrups are lifted. Lower and repeat.</t>
-  </si>
-  <si>
-    <t>Front Raise:  Alternating</t>
-  </si>
-  <si>
-    <t>Stand with low double pulleys behind. Grasp stirrup attachments, one in each hand. Stand away from pulley slightly with arms back somewhat at side and elbows straight or slightly bent.</t>
-  </si>
-  <si>
-    <t>Raise one stirrup forward and upward until upper arm is well above horizontal. Lower and repeat with opposite arm, alternating between arms.</t>
-  </si>
-  <si>
-    <t>SUNDAY</t>
-  </si>
-  <si>
-    <t>Triceps Extension</t>
-  </si>
-  <si>
-    <t>Sit on utility weight bench with barbell. Position barbell overhead with narrow overhand grip.</t>
-  </si>
-  <si>
-    <t>Lower barbell behind upper shoulders by flexing elbows allowing forearms to travel behind upper arms with elbows remaining overhead. Raise barbell overhead by extending elbows until arms are positioned straight and vertical. Lower and repeat.</t>
-  </si>
-  <si>
-    <t>Incline Shoulder Raise</t>
-  </si>
-  <si>
-    <t>Lie supine on incline bench. Dismount barbell from rack with shoulder width overhand grip. Position barbell over upper chest with elbows extended.</t>
-  </si>
-  <si>
-    <t>Pullover</t>
-  </si>
-  <si>
-    <t>Lie upper back perpendicular on bench. Flex hips slightly. Grasp barbell from behind and position over chest with elbows bent slightly.</t>
-  </si>
-  <si>
-    <t>With elbows bent slightly, lower bar over and beyond head until shoulders are fully flexed or upper arms are approximately parallel to torso. Return and repeat.</t>
-  </si>
-  <si>
-    <t>Incline Fly</t>
-  </si>
-  <si>
-    <t>Sit on seat with stirrups in each hand (attached to low cable pulleys). Lie back on incline back support. Position stirrups out to each side of chest with bent arm under each wrist. Press stirrups over each shoulder until arms vertical. Bend elbows slightly and internally rotate shoulders so elbows point out to sides.</t>
-  </si>
-  <si>
-    <t>Lower stirrups outward to sides of shoulders. Keep elbows fixed in slightly bent position. When a stretch is felt in chest or shoulders, bring stirrups back together in hugging motion above upper chest until stirrups are nearly together Repeat.</t>
-  </si>
-  <si>
-    <t>Military Press:  Seated</t>
-  </si>
-  <si>
-    <t>Grasp barbell with slightly wider than shoulder width overhand grip from rack. Position bar near upper chest.</t>
-  </si>
-  <si>
-    <t>Press bar upward until arms are extended overhead. Return to upper chest and repeat.</t>
-  </si>
-  <si>
-    <t>Upright Row</t>
-  </si>
-  <si>
-    <t>Grasp bar with shoulder width or slightly narrower overhand grip.</t>
-  </si>
-  <si>
     <t>Rear Delt Row:  Standing Rear Delt Row (stirrups)</t>
   </si>
   <si>
@@ -479,15 +578,6 @@
   </si>
   <si>
     <t>Pull stirrups out to sides, keeping elbows at shoulder height until elbows travel slightly behind back. Allow wrists to follow elbows. Keep upper arms horizontal, perpendicular to trunk. Return until arms are extended and shoulders are stretched forward. Repeat.</t>
-  </si>
-  <si>
-    <t>Front Lateral Raise</t>
-  </si>
-  <si>
-    <t>Grasp dumbbell cable attachment. Stand facing side with resting arm toward low pulley. Grasp ballet bar if available for support. Internally rotate shoulders so elbows point out to sides.</t>
-  </si>
-  <si>
-    <t>With elbow straight or slightly bent, raise upper arm away from low pulley to side, slightly to front (30°) until upper arm is shoulder height. Lower and repeat. Continue with opposite arm.</t>
   </si>
 </sst>
 </file>
@@ -852,11 +942,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -932,24 +1023,24 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -966,32 +1057,32 @@
         <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
       </c>
       <c r="D9" t="s">
         <v>36</v>
@@ -1000,7 +1091,7 @@
         <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1008,29 +1099,29 @@
         <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
         <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
         <v>43</v>
@@ -1047,7 +1138,7 @@
         <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -1064,120 +1155,120 @@
         <v>48</v>
       </c>
       <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
         <v>49</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>50</v>
       </c>
-      <c r="E15" t="s">
-        <v>51</v>
-      </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
         <v>52</v>
       </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>53</v>
       </c>
-      <c r="E16" t="s">
-        <v>54</v>
-      </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
         <v>55</v>
       </c>
-      <c r="C17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>56</v>
       </c>
-      <c r="E17" t="s">
-        <v>57</v>
-      </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F20" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="E23" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="F23" t="s">
         <v>11</v>
@@ -1185,16 +1276,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F24" t="s">
         <v>16</v>
@@ -1202,123 +1293,123 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="F25" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E26" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F26" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F27" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="F28" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="E29" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="F29" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="E30" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="F30" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="E33" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F33" t="s">
         <v>11</v>
@@ -1326,16 +1417,16 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="E34" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="F34" t="s">
         <v>16</v>
@@ -1343,123 +1434,123 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E35" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="F35" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="E36" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="F36" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="E37" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="F37" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="E38" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="F38" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="C39" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="E39" t="s">
-        <v>57</v>
+        <v>113</v>
       </c>
       <c r="F39" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="C40" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D40" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="E40" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="F40" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D43" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="E43" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="F43" t="s">
         <v>11</v>
@@ -1467,16 +1558,16 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="C44" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="E44" t="s">
-        <v>15</v>
+        <v>123</v>
       </c>
       <c r="F44" t="s">
         <v>16</v>
@@ -1484,123 +1575,123 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D45" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="E45" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="F45" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>128</v>
       </c>
       <c r="D46" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="E46" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="F46" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="D47" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="E47" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="F47" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="C48" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="E48" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="F48" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="C49" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D49" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="E49" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="F49" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="C50" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D50" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="E50" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="F50" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D53" t="s">
-        <v>82</v>
+        <v>144</v>
       </c>
       <c r="E53" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="F53" t="s">
         <v>11</v>
@@ -1608,16 +1699,16 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>52</v>
+        <v>145</v>
       </c>
       <c r="C54" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>53</v>
+        <v>146</v>
       </c>
       <c r="E54" t="s">
-        <v>54</v>
+        <v>147</v>
       </c>
       <c r="F54" t="s">
         <v>16</v>
@@ -1625,123 +1716,123 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D55" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="E55" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="F55" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="C56" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="D56" t="s">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="E56" t="s">
+        <v>104</v>
+      </c>
+      <c r="F56" t="s">
         <v>25</v>
-      </c>
-      <c r="F56" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="C57" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D57" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="E57" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="F57" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="C58" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D58" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="E58" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="F58" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="C59" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D59" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="E59" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="F59" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="C60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D60" t="s">
-        <v>131</v>
+        <v>74</v>
       </c>
       <c r="E60" t="s">
-        <v>132</v>
+        <v>75</v>
       </c>
       <c r="F60" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D63" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="E63" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="F63" t="s">
         <v>11</v>
@@ -1749,16 +1840,16 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D64" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="E64" t="s">
-        <v>47</v>
+        <v>169</v>
       </c>
       <c r="F64" t="s">
         <v>16</v>
@@ -1766,104 +1857,104 @@
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D65" t="s">
-        <v>140</v>
+        <v>171</v>
       </c>
       <c r="E65" t="s">
-        <v>141</v>
+        <v>172</v>
       </c>
       <c r="F65" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="C66" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D66" t="s">
-        <v>143</v>
+        <v>174</v>
       </c>
       <c r="E66" t="s">
-        <v>144</v>
+        <v>175</v>
       </c>
       <c r="F66" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="C67" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D67" t="s">
-        <v>146</v>
+        <v>177</v>
       </c>
       <c r="E67" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
       <c r="F67" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>148</v>
+        <v>179</v>
       </c>
       <c r="C68" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D68" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="E68" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="F68" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D69" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="E69" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="F69" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
       <c r="C70" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D70" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="E70" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="F70" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>